<commit_message>
added coal ramping parameters
</commit_message>
<xml_diff>
--- a/data/TestLocation/input_data/scenario_settings.xlsx
+++ b/data/TestLocation/input_data/scenario_settings.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25128"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/70b0e526faaa1b23/Dokumente/Alles zum Studium/Master/Masterarbeit/Leelo/data/TestLocation/input_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="35" documentId="11_AD4DB114E441178AC67DF47F8ED2CE42693EDF18" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3E5F4D45-B073-4007-88EC-811C7B63AA8E}"/>
+  <xr:revisionPtr revIDLastSave="61" documentId="11_AD4DB114E441178AC67DF47F8ED2CE42693EDF18" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8E6B50EB-1ECD-4C9D-8F9B-7AD893B56972}"/>
   <bookViews>
-    <workbookView xWindow="-8130" yWindow="-11250" windowWidth="20740" windowHeight="10750" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-6960" yWindow="-12450" windowWidth="17280" windowHeight="8960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
   <si>
     <t>n_timesteps</t>
   </si>
@@ -77,12 +77,39 @@
   </si>
   <si>
     <t>base_scenario</t>
+  </si>
+  <si>
+    <t>MinFossilShare</t>
+  </si>
+  <si>
+    <t>MaxFossilShare</t>
+  </si>
+  <si>
+    <t>Assumed</t>
+  </si>
+  <si>
+    <t>Source: A. Teruel, Perspestective of the Energy Transition: Technology Development and Investments under Uncertainty, Master thesis with DLR</t>
+  </si>
+  <si>
+    <t>euros/MW</t>
+  </si>
+  <si>
+    <t>CoalRampingHourly</t>
+  </si>
+  <si>
+    <t>CoalRampingDaily</t>
+  </si>
+  <si>
+    <t>CoalRampingWearTear</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -112,8 +139,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -394,10 +422,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:N5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -411,9 +439,14 @@
     <col min="7" max="7" width="11" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12.6640625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11.77734375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.21875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="20.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -441,8 +474,23 @@
       <c r="I1" t="s">
         <v>7</v>
       </c>
+      <c r="J1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K1" t="s">
+        <v>15</v>
+      </c>
+      <c r="L1" t="s">
+        <v>19</v>
+      </c>
+      <c r="M1" t="s">
+        <v>20</v>
+      </c>
+      <c r="N1" t="s">
+        <v>21</v>
+      </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>8760</v>
       </c>
@@ -470,8 +518,23 @@
       <c r="I2">
         <v>0.05</v>
       </c>
+      <c r="J2" s="1">
+        <v>0</v>
+      </c>
+      <c r="K2" s="1">
+        <v>1</v>
+      </c>
+      <c r="L2">
+        <v>0.1</v>
+      </c>
+      <c r="M2">
+        <v>0.1</v>
+      </c>
+      <c r="N2">
+        <v>3.3</v>
+      </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>9</v>
       </c>
@@ -480,6 +543,26 @@
       </c>
       <c r="I4" t="s">
         <v>11</v>
+      </c>
+      <c r="L4" t="s">
+        <v>18</v>
+      </c>
+      <c r="M4" t="s">
+        <v>18</v>
+      </c>
+      <c r="N4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="L5" t="s">
+        <v>16</v>
+      </c>
+      <c r="M5" t="s">
+        <v>16</v>
+      </c>
+      <c r="N5" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>